<commit_message>
updated to not work with wrong data
</commit_message>
<xml_diff>
--- a/server/data/share.xlsx
+++ b/server/data/share.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\nepse-analysis\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D6E287-C935-455C-B829-CEA512C4AE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BF7FFB-D3F5-4DD9-BAF9-41305E64C151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1202,7 +1202,7 @@
   <dimension ref="A1:U236"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="G242" sqref="G242"/>
+      <selection activeCell="G241" sqref="G241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>